<commit_message>
changed xl for testing
</commit_message>
<xml_diff>
--- a/cdss_database_v7.xlsx
+++ b/cdss_database_v7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python projects\cdss\mini-project-cdss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1A434C-88BC-4A8D-9798-E96707492FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C258B93-EEBE-4BA6-8E32-0BFAEB871964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient_Demographics" sheetId="1" r:id="rId1"/>
@@ -974,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2168,9 +2168,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1163"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="38.25" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="19.125" customWidth="1"/>
+    <col min="8" max="8" width="21.625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -32422,6 +32431,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="19.375" customWidth="1"/>
+    <col min="4" max="4" width="24.875" customWidth="1"/>
+    <col min="5" max="5" width="22.375" customWidth="1"/>
+    <col min="6" max="6" width="22.25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
added patient with recommendation
</commit_message>
<xml_diff>
--- a/cdss_database_v7.xlsx
+++ b/cdss_database_v7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python projects\cdss\mini-project-cdss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4477420-9A8E-439A-9893-2A601D862F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6B38C9-63B1-4744-8722-DF3A3B95189B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2169,7 +2169,7 @@
   <dimension ref="A1:H1162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2608,19 +2608,19 @@
         <v>169</v>
       </c>
       <c r="D17">
-        <v>36.6</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
         <v>172</v>
       </c>
       <c r="F17" s="2">
-        <v>45821.431539520927</v>
+        <v>45831.431539351855</v>
       </c>
       <c r="G17" s="2">
-        <v>45821.391539520933</v>
+        <v>45831.391539351855</v>
       </c>
       <c r="H17" s="2">
-        <v>45821.681539520927</v>
+        <v>45831.681539351855</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -32403,7 +32403,7 @@
   <dimension ref="A1:F808"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -32744,7 +32744,7 @@
         <v>177</v>
       </c>
       <c r="C17" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D17" s="2">
         <v>45832.981006944443</v>

</xml_diff>

<commit_message>
added some temps to the excel and changed its before after to 1 day
</commit_message>
<xml_diff>
--- a/cdss_database_v7.xlsx
+++ b/cdss_database_v7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python projects\cdss\mini-project-cdss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B7511C-B3B7-4806-AD2B-CC42733CED78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D6769D-D777-4C20-A514-E17EB7E93950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient_Demographics" sheetId="1" r:id="rId1"/>
@@ -974,7 +974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -2168,8 +2168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A488" workbookViewId="0">
-      <selection activeCell="J508" sqref="J508"/>
+    <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3134,13 +3134,13 @@
         <v>172</v>
       </c>
       <c r="F37" s="2">
-        <v>45812.385391724201</v>
+        <v>45831.385393518518</v>
       </c>
       <c r="G37" s="2">
-        <v>45812.3453917242</v>
+        <v>45831.345393518517</v>
       </c>
       <c r="H37" s="2">
-        <v>45812.635391724201</v>
+        <v>45831.635393518518</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -15712,19 +15712,19 @@
         <v>169</v>
       </c>
       <c r="D521">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E521" t="s">
         <v>172</v>
       </c>
       <c r="F521" s="2">
-        <v>45822.828424357918</v>
+        <v>45831.411759259259</v>
       </c>
       <c r="G521" s="2">
-        <v>45822.788424357917</v>
+        <v>45831.371759259258</v>
       </c>
       <c r="H521" s="2">
-        <v>45823.078424357918</v>
+        <v>45832.078425925924</v>
       </c>
     </row>
     <row r="522" spans="1:8" x14ac:dyDescent="0.2">
@@ -32402,8 +32402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F805"/>
   <sheetViews>
-    <sheetView topLeftCell="A194" workbookViewId="0">
-      <selection activeCell="E206" sqref="E206"/>
+    <sheetView topLeftCell="A598" workbookViewId="0">
+      <selection activeCell="C629" sqref="C629"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
upload DB last time
</commit_message>
<xml_diff>
--- a/cdss_database_v7.xlsx
+++ b/cdss_database_v7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python projects\cdss\mini-project-cdss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BDB14F-1C77-4F9C-9A9D-1E9BDB72EA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C2EC4F-90E5-4FF2-811D-D15A2F44BF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32403,7 +32403,7 @@
   <dimension ref="A1:F805"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A353" workbookViewId="0">
-      <selection activeCell="D364" sqref="D364"/>
+      <selection activeCell="E365" sqref="E365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -39707,7 +39707,7 @@
         <v>181</v>
       </c>
       <c r="D365" s="2">
-        <v>45815.752405833278</v>
+        <v>45815.753101851849</v>
       </c>
       <c r="E365" s="2">
         <v>45815.502405833278</v>

</xml_diff>